<commit_message>
listas de requesitos atualizada
</commit_message>
<xml_diff>
--- a/ListaDeRaquesitos.xlsx
+++ b/ListaDeRaquesitos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heliveltontavares\Google Drive\Trabalho de  conclusao de curso\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Requesitos" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>Cod. Requisito</t>
   </si>
@@ -229,6 +224,81 @@
   </si>
   <si>
     <t>O sistema deverá permitir que, para cada unidade de ensino, seja cadastrada  nome, telefone, endereco e  sigla.</t>
+  </si>
+  <si>
+    <t>RNF02</t>
+  </si>
+  <si>
+    <t>O tempo de execução</t>
+  </si>
+  <si>
+    <t>O sistema deverá verificar se o usuário esta mais de 4 minutos logado sem nenhuma ação, o sistema devera após devera emitir um alerta de inativade.</t>
+  </si>
+  <si>
+    <t>RNF03</t>
+  </si>
+  <si>
+    <t>RNF04</t>
+  </si>
+  <si>
+    <t>RNF05</t>
+  </si>
+  <si>
+    <t>RNF06</t>
+  </si>
+  <si>
+    <t>RNF07</t>
+  </si>
+  <si>
+    <t>RNF08</t>
+  </si>
+  <si>
+    <t>RNF09</t>
+  </si>
+  <si>
+    <t>RNF10</t>
+  </si>
+  <si>
+    <t>O sistema operacional do sistema</t>
+  </si>
+  <si>
+    <t>O sistema deverá ser acessado por varios tipos de sistemas operacionais ao mesmo tempo.</t>
+  </si>
+  <si>
+    <t>O desenvolvimento do sistema</t>
+  </si>
+  <si>
+    <t>O sistema deverá ser desenvolvido ele toda em linguagem de programação JAVA</t>
+  </si>
+  <si>
+    <t>Banco de dados do sistema</t>
+  </si>
+  <si>
+    <t>O sistema devera se comunicar com o Banco de Dados Postgree</t>
+  </si>
+  <si>
+    <t>Intregação com outro sistema</t>
+  </si>
+  <si>
+    <t>O sistema deverá ser feito que possibilite a intregração com outro sistema.</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter alta disponibilidade</t>
+  </si>
+  <si>
+    <t>O sistema deverá ter alta disponibilidade, por exemplo 99% do tempo.</t>
+  </si>
+  <si>
+    <t>Tempo de processamento</t>
+  </si>
+  <si>
+    <t>O sistema deverá processo N requisições por um determinado tempo.</t>
+  </si>
+  <si>
+    <t>Confiabilidade</t>
+  </si>
+  <si>
+    <t>O sistema não deverá apresentar aos usuários quaisquer dados de cunho privativo.</t>
   </si>
 </sst>
 </file>
@@ -280,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -353,20 +423,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -403,16 +464,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -482,7 +533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,7 +568,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -702,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="99" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,12 +1084,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1354,17 +1405,128 @@
       </c>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="13"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="13"/>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="13"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>